<commit_message>
Answered questions to homework
</commit_message>
<xml_diff>
--- a/Macro Ecnomics/PP Assignment 1.xlsx
+++ b/Macro Ecnomics/PP Assignment 1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>A</t>
   </si>
@@ -38,14 +38,106 @@
   </si>
   <si>
     <t>Bread</t>
+  </si>
+  <si>
+    <t>Data Set</t>
+  </si>
+  <si>
+    <t>Plot Point</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="24"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Author: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="24"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Chuck Reeves</t>
+    </r>
+  </si>
+  <si>
+    <t>Questions about the table above.</t>
+  </si>
+  <si>
+    <t>1) In choice A if we use all of our scarce resources to produce bread, what happens to the production of tractors?</t>
+  </si>
+  <si>
+    <t>2) Since tractors are a symbol for capital goods, what does this imply for the future?</t>
+  </si>
+  <si>
+    <t>3) In choice F if we use all of our scarce resources to produce tractors, what happens to the production of bread?</t>
+  </si>
+  <si>
+    <t>4) Since bread is a symbol for consumer goods, what does this imply for the future?</t>
+  </si>
+  <si>
+    <t>5) What is the best choice? (this is a trick question)</t>
+  </si>
+  <si>
+    <t>6) How is a choice made? (not a trick question)</t>
+  </si>
+  <si>
+    <t>The opportunity cost of Tractors increases due to resources being allocated to Bread</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The opportunity cost of Bread increases </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> a larger production of consumer goods</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A decrease in capital goods </t>
+  </si>
+  <si>
+    <t>Choice C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Investing in Capital goods will help the economy grown and provide an increase in Consumer goods </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="4">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="24"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="24"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -61,7 +153,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -69,12 +161,111 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -108,8 +299,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.11062987992642652"/>
-          <c:y val="1.666666666666667E-2"/>
+          <c:x val="0.11272961745923492"/>
+          <c:y val="0"/>
         </c:manualLayout>
       </c:layout>
     </c:title>
@@ -122,7 +313,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'PRODUCTION POSSIBILITIES '!$C$1</c:f>
+              <c:f>'PRODUCTION POSSIBILITIES '!$D$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -294,7 +485,7 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>'PRODUCTION POSSIBILITIES '!$B$2:$B$7</c:f>
+              <c:f>'PRODUCTION POSSIBILITIES '!$C$6:$C$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -321,7 +512,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'PRODUCTION POSSIBILITIES '!$C$2:$C$7</c:f>
+              <c:f>'PRODUCTION POSSIBILITIES '!$D$6:$D$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -351,11 +542,11 @@
         <c:dLbls>
           <c:showVal val="1"/>
         </c:dLbls>
-        <c:axId val="64543744"/>
-        <c:axId val="64551552"/>
+        <c:axId val="65272064"/>
+        <c:axId val="87496576"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="64543744"/>
+        <c:axId val="65272064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -381,7 +572,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64551552"/>
+        <c:crossAx val="87496576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:dispUnits>
@@ -392,7 +583,7 @@
         </c:dispUnits>
       </c:valAx>
       <c:valAx>
-        <c:axId val="64551552"/>
+        <c:axId val="87496576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -418,7 +609,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64543744"/>
+        <c:crossAx val="65272064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:dispUnits>
@@ -442,7 +633,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -452,16 +643,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -768,90 +959,181 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="B1" t="s">
+    <row r="1" spans="1:5" ht="31.5">
+      <c r="A1" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" thickBot="1"/>
+    <row r="4" spans="1:5">
+      <c r="B4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="3"/>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="B5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D5" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
+    <row r="6" spans="1:5">
+      <c r="B6" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2">
+      <c r="C6" s="5">
         <v>0</v>
       </c>
-      <c r="C2">
+      <c r="D6" s="6">
         <v>30000</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
+    <row r="7" spans="1:5">
+      <c r="B7" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B3">
+      <c r="C7" s="5">
         <v>1000</v>
       </c>
-      <c r="C3">
+      <c r="D7" s="6">
         <v>28000</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
+    <row r="8" spans="1:5">
+      <c r="B8" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B4">
+      <c r="C8" s="5">
         <v>2000</v>
       </c>
-      <c r="C4">
+      <c r="D8" s="6">
         <v>24000</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
+    <row r="9" spans="1:5">
+      <c r="B9" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5">
+      <c r="C9" s="5">
         <v>3000</v>
       </c>
-      <c r="C5">
+      <c r="D9" s="6">
         <v>18000</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
+    <row r="10" spans="1:5">
+      <c r="B10" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B6">
+      <c r="C10" s="5">
         <v>4000</v>
       </c>
-      <c r="C6">
+      <c r="D10" s="6">
         <v>10000</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
+    <row r="11" spans="1:5" ht="15.75" thickBot="1">
+      <c r="B11" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B7">
+      <c r="C11" s="8">
         <v>5000</v>
       </c>
-      <c r="C7">
+      <c r="D11" s="9">
         <v>0</v>
       </c>
     </row>
+    <row r="25" spans="1:1">
+      <c r="A25" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" ht="14.25" customHeight="1">
+      <c r="A35" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" ht="14.25" customHeight="1">
+      <c r="A36" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" ht="14.25" customHeight="1"/>
+    <row r="38" spans="1:1">
+      <c r="A38" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Dicussion number 2 DER
</commit_message>
<xml_diff>
--- a/Macro Ecnomics/PP Assignment 1.xlsx
+++ b/Macro Ecnomics/PP Assignment 1.xlsx
@@ -38,9 +38,6 @@
   </si>
   <si>
     <t>Bread</t>
-  </si>
-  <si>
-    <t>Data Set</t>
   </si>
   <si>
     <t>Plot Point</t>
@@ -107,12 +104,15 @@
   <si>
     <t xml:space="preserve">Investing in Capital goods will help the economy grown and provide an increase in Consumer goods </t>
   </si>
+  <si>
+    <t>Data Table</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -137,6 +137,14 @@
     </font>
     <font>
       <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color theme="1"/>
@@ -245,8 +253,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -256,16 +272,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -299,7 +308,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.11272961745923492"/>
+          <c:x val="0.11272961745923495"/>
           <c:y val="0"/>
         </c:manualLayout>
       </c:layout>
@@ -542,11 +551,11 @@
         <c:dLbls>
           <c:showVal val="1"/>
         </c:dLbls>
-        <c:axId val="65272064"/>
-        <c:axId val="87496576"/>
+        <c:axId val="73054848"/>
+        <c:axId val="73062272"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="65272064"/>
+        <c:axId val="73054848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -562,9 +571,10 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Tractors</a:t>
+                  <a:rPr lang="en-US" sz="1000" b="1" i="0" u="none" strike="noStrike" baseline="0"/>
+                  <a:t>Tractors (000s)</a:t>
                 </a:r>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -572,7 +582,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87496576"/>
+        <c:crossAx val="73062272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:dispUnits>
@@ -583,7 +593,7 @@
         </c:dispUnits>
       </c:valAx>
       <c:valAx>
-        <c:axId val="87496576"/>
+        <c:axId val="73062272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -599,9 +609,10 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Bread</a:t>
+                  <a:rPr lang="en-US" sz="1000" b="1" i="0" u="none" strike="noStrike" baseline="0"/>
+                  <a:t>Bread (000,000s of loaves)</a:t>
                 </a:r>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -609,7 +620,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="65272064"/>
+        <c:crossAx val="73054848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:dispUnits>
@@ -633,7 +644,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -959,173 +970,176 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:5" ht="31.5">
-      <c r="A1" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
+      <c r="A1" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" thickBot="1"/>
     <row r="4" spans="1:5">
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="10"/>
+      <c r="D4" s="11"/>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="3"/>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="B5" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="2">
         <v>0</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="3">
         <v>30000</v>
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="2">
         <v>1000</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="3">
         <v>28000</v>
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="2">
         <v>2000</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="3">
         <v>24000</v>
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="2">
         <v>3000</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="3">
         <v>18000</v>
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="2">
         <v>4000</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="3">
         <v>10000</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15.75" thickBot="1">
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="8">
+      <c r="C11" s="5">
         <v>5000</v>
       </c>
-      <c r="D11" s="9">
+      <c r="D11" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:1">
-      <c r="A25" s="11" t="s">
-        <v>11</v>
+      <c r="A25" s="7" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="35" spans="1:1" ht="14.25" customHeight="1">
       <c r="A35" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="36" spans="1:1" ht="14.25" customHeight="1">
       <c r="A36" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="37" spans="1:1" ht="14.25" customHeight="1"/>
     <row r="38" spans="1:1">
       <c r="A38" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="42" spans="1:1">
       <c r="A42" t="s">
-        <v>23</v>
-      </c>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1">
+      <c r="A44" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>